<commit_message>
Fixed the problem of peak longitudinal acceleration in the start
Tried running Budapest
</commit_message>
<xml_diff>
--- a/+Model/LLTD_sweep.xlsx
+++ b/+Model/LLTD_sweep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\LaptimeSimOCP\+Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\LaptimeSimOCP\+Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C3F20-E734-4B1B-B2E4-259268217AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B227B55-9FBE-4F23-AF1F-676315548E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="756" windowWidth="21660" windowHeight="11328" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="MassInertia" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>setup</t>
   </si>
@@ -178,13 +178,19 @@
     <t>maximum_torque</t>
   </si>
   <si>
-    <t>"-5% lltd"</t>
-  </si>
-  <si>
-    <t>"-15% lltd"</t>
-  </si>
-  <si>
-    <t>"-10% lltd"</t>
+    <t>gear_ratio</t>
+  </si>
+  <si>
+    <t>GearRatio.xlsx</t>
+  </si>
+  <si>
+    <t>3 lltd</t>
+  </si>
+  <si>
+    <t>6 lltd</t>
+  </si>
+  <si>
+    <t>9 lltd</t>
   </si>
 </sst>
 </file>
@@ -539,16 +545,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E820AE81-6940-42C1-9794-755A660CF3D0}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -619,12 +625,12 @@
         <v>9.8059999999999992</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>965</v>
@@ -648,19 +654,19 @@
         <v>0.316</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J5" si="0">0.47</f>
+        <f>0.47</f>
         <v>0.47</v>
       </c>
       <c r="K3">
         <v>9.8059999999999992</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>965</v>
@@ -684,19 +690,19 @@
         <v>0.316</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f>0.47</f>
         <v>0.47</v>
       </c>
       <c r="K4">
         <v>9.8059999999999992</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C5">
         <v>965</v>
@@ -720,7 +726,7 @@
         <v>0.316</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f>0.47</f>
         <v>0.47</v>
       </c>
       <c r="K5">
@@ -734,21 +740,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438D574D-38FE-45DB-9CEC-921C97E214E2}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -761,61 +768,76 @@
       <c r="D1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -832,13 +854,13 @@
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -849,7 +871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3.0049999999999999</v>
       </c>
@@ -860,7 +882,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3.0049999999999999</v>
       </c>
@@ -871,7 +893,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3.0049999999999999</v>
       </c>
@@ -882,7 +904,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.0049999999999999</v>
       </c>
@@ -903,12 +925,12 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I5"/>
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -937,7 +959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -966,7 +988,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -995,7 +1017,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1024,7 +1046,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1063,13 +1085,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9507F4BD-F65E-43DC-B9A6-0DFC5F26B653}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1086,12 +1108,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.0029999999999999</v>
       </c>
       <c r="B2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C2">
         <v>1.2250000000000001</v>
@@ -1104,54 +1126,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.0029999999999999</v>
       </c>
       <c r="B3">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C3">
         <v>1.2250000000000001</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D5" si="0">44/100</f>
+        <f>44/100</f>
         <v>0.44</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.0029999999999999</v>
       </c>
       <c r="B4">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C4">
         <v>1.2250000000000001</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>44/100</f>
         <v>0.44</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.0029999999999999</v>
       </c>
       <c r="B5">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C5">
         <v>1.2250000000000001</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>44/100</f>
         <v>0.44</v>
       </c>
       <c r="E5">
@@ -1171,32 +1193,31 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>60/100</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.45</v>
+        <v>0.59</v>
       </c>
     </row>
   </sheetData>
@@ -1209,15 +1230,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1228,7 +1249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -1239,7 +1260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2E-3</v>
       </c>
@@ -1250,7 +1271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2E-3</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2E-3</v>
       </c>
@@ -1282,15 +1303,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1301,7 +1322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -1312,7 +1333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2E-3</v>
       </c>
@@ -1323,7 +1344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2E-3</v>
       </c>
@@ -1334,7 +1355,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2E-3</v>
       </c>
@@ -1355,15 +1376,15 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1371,40 +1392,40 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0.7</f>
         <v>0.7</v>
       </c>
       <c r="B2" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f t="shared" ref="A3:A5" si="0">0.7</f>
+        <f>0.7</f>
         <v>0.7</v>
       </c>
       <c r="B3" s="1">
-        <v>5001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" si="0"/>
+        <f>0.7</f>
         <v>0.7</v>
       </c>
       <c r="B4" s="1">
-        <v>5002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f>0.7</f>
         <v>0.7</v>
       </c>
       <c r="B5" s="1">
-        <v>5003</v>
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
@@ -1418,12 +1439,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1431,7 +1452,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>50</v>
       </c>
@@ -1439,7 +1460,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>50</v>
       </c>
@@ -1447,7 +1468,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>50</v>
       </c>
@@ -1455,7 +1476,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
added constraints on understeer angle and beta angle maximum value
started to investigate the implementation of interpolation inside casadi
</commit_message>
<xml_diff>
--- a/+Model/LLTD_sweep.xlsx
+++ b/+Model/LLTD_sweep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\LaptimeSimOCP\+Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B227B55-9FBE-4F23-AF1F-676315548E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DB6171-4065-45CD-A5E1-F3D615305A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="MassInertia" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>setup</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>9 lltd</t>
+  </si>
+  <si>
+    <t>12 lltd</t>
   </si>
 </sst>
 </file>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E820AE81-6940-42C1-9794-755A660CF3D0}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +618,7 @@
         <v>4.4939999999999998</v>
       </c>
       <c r="I2">
-        <v>0.316</v>
+        <v>0.4</v>
       </c>
       <c r="J2">
         <f>0.47</f>
@@ -651,7 +654,7 @@
         <v>4.4939999999999998</v>
       </c>
       <c r="I3">
-        <v>0.316</v>
+        <v>0.4</v>
       </c>
       <c r="J3">
         <f>0.47</f>
@@ -687,7 +690,7 @@
         <v>4.4939999999999998</v>
       </c>
       <c r="I4">
-        <v>0.316</v>
+        <v>0.4</v>
       </c>
       <c r="J4">
         <f>0.47</f>
@@ -723,13 +726,49 @@
         <v>4.4939999999999998</v>
       </c>
       <c r="I5">
-        <v>0.316</v>
+        <v>0.4</v>
       </c>
       <c r="J5">
         <f>0.47</f>
         <v>0.47</v>
       </c>
       <c r="K5">
+        <v>9.8059999999999992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>965</v>
+      </c>
+      <c r="D6">
+        <v>1400</v>
+      </c>
+      <c r="E6">
+        <v>3.7050000000000001</v>
+      </c>
+      <c r="F6">
+        <v>3.7050000000000001</v>
+      </c>
+      <c r="G6">
+        <v>4.4939999999999998</v>
+      </c>
+      <c r="H6">
+        <v>4.4939999999999998</v>
+      </c>
+      <c r="I6">
+        <v>0.4</v>
+      </c>
+      <c r="J6">
+        <f>0.47</f>
+        <v>0.47</v>
+      </c>
+      <c r="K6">
         <v>9.8059999999999992</v>
       </c>
     </row>
@@ -740,10 +779,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438D574D-38FE-45DB-9CEC-921C97E214E2}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,6 +879,23 @@
         <v>45</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3.5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>550</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -848,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901643AF-9B68-41E5-8036-1B2EA82A4089}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,6 +971,17 @@
         <v>1.55</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="B6">
+        <v>1.56</v>
+      </c>
+      <c r="C6">
+        <v>1.55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -922,10 +989,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931E2177-CC67-45BC-8CE0-3909A4C3BCE5}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
+      <selection activeCell="A6" sqref="A6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,6 +1139,35 @@
         <v>0</v>
       </c>
       <c r="I5">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>13.7</v>
       </c>
     </row>
@@ -1083,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9507F4BD-F65E-43DC-B9A6-0DFC5F26B653}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,7 +1209,7 @@
         <v>1.0029999999999999</v>
       </c>
       <c r="B2">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1.2250000000000001</v>
@@ -1131,7 +1227,7 @@
         <v>1.0029999999999999</v>
       </c>
       <c r="B3">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1.2250000000000001</v>
@@ -1149,7 +1245,7 @@
         <v>1.0029999999999999</v>
       </c>
       <c r="B4">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1.2250000000000001</v>
@@ -1167,7 +1263,7 @@
         <v>1.0029999999999999</v>
       </c>
       <c r="B5">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1.2250000000000001</v>
@@ -1177,6 +1273,24 @@
         <v>0.44</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D6">
+        <f>44/100</f>
+        <v>0.44</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
     </row>
@@ -1187,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFC2CF-704D-43BE-8FC5-847EC40E2F8A}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,6 +1334,11 @@
         <v>0.59</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1227,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2744984F-2619-4555-ADE9-32DB97027A3A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1293,6 +1412,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2E-3</v>
+      </c>
+      <c r="B6">
+        <v>0.33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1300,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FB8345-2836-4EBD-AAF9-7C5C9AEC5DDE}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,6 +1496,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2E-3</v>
+      </c>
+      <c r="B6">
+        <v>0.33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1373,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E935BBC8-6905-40C4-93AA-35113AE6796F}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1428,6 +1569,15 @@
         <v>8000</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>0.7</f>
+        <v>0.7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1436,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6950B1FE-C003-4061-B478-DBB29EFBCD69}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1484,6 +1634,14 @@
         <v>1.8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>1.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>